<commit_message>
adicinaram se metodos bugados
</commit_message>
<xml_diff>
--- a/resultados/Resultados.xlsx
+++ b/resultados/Resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FabioS\Desktop\2021-22\TI\TP2\resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064B28B1-7C29-4CE8-84A4-EAE22030D58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E31CE2-B9CB-4D5E-83ED-AA73D98A814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5256" yWindow="1896" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Métodos de compressão</t>
   </si>
@@ -46,6 +46,27 @@
   </si>
   <si>
     <t>ORIGINAL (kbytes)</t>
+  </si>
+  <si>
+    <t>Huffman</t>
+  </si>
+  <si>
+    <t>LZW</t>
+  </si>
+  <si>
+    <t>PPM</t>
+  </si>
+  <si>
+    <t>decoders: +30kb</t>
+  </si>
+  <si>
+    <t>decoders igual</t>
+  </si>
+  <si>
+    <t>decoders: +9kb</t>
+  </si>
+  <si>
+    <t>bz2 fica diferente</t>
   </si>
 </sst>
 </file>
@@ -117,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -134,7 +155,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -417,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,25 +506,55 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2167</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3703</v>
+      </c>
+      <c r="D4" s="5">
+        <v>180</v>
+      </c>
+      <c r="E4" s="6">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
+        <v>730</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1315</v>
+      </c>
+      <c r="D5" s="5">
+        <v>172</v>
+      </c>
+      <c r="E5" s="5">
+        <v>144</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>730</v>
+      </c>
+      <c r="C6" s="5">
+        <v>177</v>
+      </c>
+      <c r="D6" s="5">
+        <v>61</v>
+      </c>
+      <c r="E6" s="5">
+        <v>76</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
@@ -530,6 +584,28 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>